<commit_message>
V1.0_Patch_01 arreglos de duplicado de operadora, error en supervisor, quitar read_only de formularios, etc
</commit_message>
<xml_diff>
--- a/geo_certifications/security/generador_permisos.xlsx
+++ b/geo_certifications/security/generador_permisos.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="43">
   <si>
     <t>vehicle_for_administrator</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>certifications_administrator</t>
+  </si>
+  <si>
+    <t>certification_contract</t>
   </si>
 </sst>
 </file>
@@ -483,7 +486,7 @@
   <dimension ref="A1:J54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -737,9 +740,18 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" t="s">
+        <v>41</v>
+      </c>
       <c r="E15" t="str">
         <f>CONCATENATE(Datos!A10,",",Datos!B10,",",Datos!C10,",",Datos!D10,",",Datos!E10,",",Datos!F10,",",Datos!G10,",",Datos!H10)</f>
-        <v>access__for_group_name_,_for_,model_,group_name_,0,0,0,0</v>
+        <v>access_certification_contract_for_group_name_certifications_administrator,certification_contract_for_certifications_administrator,model_certification_contract,group_name_certifications_administrator,1,1,1,1</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1366,35 +1378,35 @@
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>CONCATENATE("access_",Permisos!B15,"_for_","group_name_",Permisos!D15)</f>
-        <v>access__for_group_name_</v>
+        <v>access_certification_contract_for_group_name_certifications_administrator</v>
       </c>
       <c r="B10" t="str">
         <f>CONCATENATE(Permisos!B15,"_for_",Permisos!D15)</f>
-        <v>_for_</v>
+        <v>certification_contract_for_certifications_administrator</v>
       </c>
       <c r="C10" t="str">
         <f>CONCATENATE("model_",Permisos!B15)</f>
-        <v>model_</v>
+        <v>model_certification_contract</v>
       </c>
       <c r="D10" t="str">
         <f>CONCATENATE("group_name_",Permisos!D15)</f>
-        <v>group_name_</v>
+        <v>group_name_certifications_administrator</v>
       </c>
       <c r="E10" t="str">
         <f>IF(ISNUMBER(SEARCH("read",Permisos!$C15)),"1","0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" t="str">
         <f>IF(ISNUMBER(SEARCH("write",Permisos!$C15)),"1","0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" t="str">
         <f>IF(ISNUMBER(SEARCH("create",Permisos!$C15)),"1","0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" t="str">
         <f>IF(ISNUMBER(SEARCH("unlink",Permisos!$C15)),"1","0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Modificaciones iniciales de seguridad
</commit_message>
<xml_diff>
--- a/geo_certifications/security/generador_permisos.xlsx
+++ b/geo_certifications/security/generador_permisos.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="45">
   <si>
     <t>vehicle_for_administrator</t>
   </si>
@@ -27,124 +27,130 @@
     <t>vehicle_model_for_administrator</t>
   </si>
   <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>model_id:id</t>
+  </si>
+  <si>
+    <t>group_id:id</t>
+  </si>
+  <si>
+    <t>perm_read</t>
+  </si>
+  <si>
+    <t>perm_write</t>
+  </si>
+  <si>
+    <t>perm_create</t>
+  </si>
+  <si>
+    <t>perm_unlink</t>
+  </si>
+  <si>
+    <t>Modelo</t>
+  </si>
+  <si>
+    <t>Calculo</t>
+  </si>
+  <si>
+    <t>Permiso (r,u,c,d)</t>
+  </si>
+  <si>
+    <t>Group_name</t>
+  </si>
+  <si>
+    <t>read_write_create_unlink</t>
+  </si>
+  <si>
+    <t>app base</t>
+  </si>
+  <si>
+    <t>model_certifications.certification_ceyf</t>
+  </si>
+  <si>
+    <t>model_certifications.certification</t>
+  </si>
+  <si>
+    <t>model_certifications.certification_coiled_tubing</t>
+  </si>
+  <si>
+    <t>model_certifications.coiled_tubing_time_losed</t>
+  </si>
+  <si>
+    <t>group_name_certification_administrator</t>
+  </si>
+  <si>
+    <t>access_certification_for_administrator</t>
+  </si>
+  <si>
+    <t>access_certification_ceyf_for_administrator</t>
+  </si>
+  <si>
+    <t>access_certification_coiled_tubing_for_administrator</t>
+  </si>
+  <si>
+    <t>access_coiled_tubing_time_losed_for_administrator</t>
+  </si>
+  <si>
+    <t>certifications_certification</t>
+  </si>
+  <si>
+    <t>certifications_certification_ceyf</t>
+  </si>
+  <si>
+    <t>certifications_certification_coiled_tubing</t>
+  </si>
+  <si>
+    <t>certifications_coiled_tubing_time_losed</t>
+  </si>
+  <si>
+    <t>certifications_certification_task</t>
+  </si>
+  <si>
+    <t>certifications_certification_task_stage</t>
+  </si>
+  <si>
+    <t>certification_invoice</t>
+  </si>
+  <si>
+    <t>certifications_supervisor</t>
+  </si>
+  <si>
+    <t>certifications_administrator</t>
+  </si>
+  <si>
+    <t>certification_contract</t>
+  </si>
+  <si>
+    <t>certifications_ingenieria</t>
+  </si>
+  <si>
+    <t>certifications_administracion</t>
+  </si>
+  <si>
     <t>read</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>model_id:id</t>
-  </si>
-  <si>
-    <t>group_id:id</t>
-  </si>
-  <si>
-    <t>perm_read</t>
-  </si>
-  <si>
-    <t>perm_write</t>
-  </si>
-  <si>
-    <t>perm_create</t>
-  </si>
-  <si>
-    <t>perm_unlink</t>
-  </si>
-  <si>
-    <t>Modelo</t>
-  </si>
-  <si>
-    <t>Calculo</t>
-  </si>
-  <si>
-    <t>Permiso (r,u,c,d)</t>
-  </si>
-  <si>
-    <t>Group_name</t>
-  </si>
-  <si>
-    <t>read_write_create_unlink</t>
-  </si>
-  <si>
-    <t>app base</t>
-  </si>
-  <si>
-    <t>vehicle</t>
-  </si>
-  <si>
-    <t>vehicle_model</t>
-  </si>
-  <si>
-    <t>vehicle_color</t>
-  </si>
-  <si>
-    <t>vehicle_status</t>
-  </si>
-  <si>
-    <t>res_partner</t>
-  </si>
-  <si>
-    <t>config</t>
-  </si>
-  <si>
-    <t>model_certifications.certification_ceyf</t>
-  </si>
-  <si>
-    <t>model_certifications.certification</t>
-  </si>
-  <si>
-    <t>model_certifications.certification_coiled_tubing</t>
-  </si>
-  <si>
-    <t>model_certifications.coiled_tubing_time_losed</t>
-  </si>
-  <si>
-    <t>group_name_certification_administrator</t>
-  </si>
-  <si>
-    <t>access_certification_for_administrator</t>
-  </si>
-  <si>
-    <t>access_certification_ceyf_for_administrator</t>
-  </si>
-  <si>
-    <t>access_certification_coiled_tubing_for_administrator</t>
-  </si>
-  <si>
-    <t>access_coiled_tubing_time_losed_for_administrator</t>
-  </si>
-  <si>
-    <t>certifications_certification</t>
-  </si>
-  <si>
-    <t>certifications_certification_ceyf</t>
-  </si>
-  <si>
-    <t>certifications_certification_coiled_tubing</t>
-  </si>
-  <si>
-    <t>certifications_coiled_tubing_time_losed</t>
-  </si>
-  <si>
-    <t>certifications_certification_task</t>
-  </si>
-  <si>
-    <t>certifications_certification_task_stage</t>
-  </si>
-  <si>
-    <t>certification_invoice</t>
-  </si>
-  <si>
-    <t>certifications_supervisor</t>
-  </si>
-  <si>
-    <t>certifications_administrator</t>
-  </si>
-  <si>
-    <t>certification_contract</t>
+    <t>read_write</t>
+  </si>
+  <si>
+    <t>read_write_create</t>
+  </si>
+  <si>
+    <t>exchange_administrator</t>
+  </si>
+  <si>
+    <t>exchange_administracion</t>
+  </si>
+  <si>
+    <t>solo_lectura</t>
+  </si>
+  <si>
+    <t>exchange_cotizacion_dolar_bcra</t>
   </si>
 </sst>
 </file>
@@ -485,8 +491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,16 +506,16 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="F1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="G1">
         <v>1</v>
@@ -526,16 +532,16 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="F2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -552,16 +558,16 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -578,16 +584,16 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -604,30 +610,30 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
         <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E7" t="str">
         <f>CONCATENATE(Datos!A2,",",Datos!B2,",",Datos!C2,",",Datos!D2,",",Datos!E2,",",Datos!F2,",",Datos!G2,",",Datos!H2)</f>
@@ -636,13 +642,13 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
         <v>34</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" t="s">
-        <v>41</v>
       </c>
       <c r="E8" t="str">
         <f>CONCATENATE(Datos!A3,",",Datos!B3,",",Datos!C3,",",Datos!D3,",",Datos!E3,",",Datos!F3,",",Datos!G3,",",Datos!H3)</f>
@@ -651,13 +657,13 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E9" t="str">
         <f>CONCATENATE(Datos!A4,",",Datos!B4,",",Datos!C4,",",Datos!D4,",",Datos!E4,",",Datos!F4,",",Datos!G4,",",Datos!H4)</f>
@@ -666,13 +672,13 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E10" t="str">
         <f>CONCATENATE(Datos!A5,",",Datos!B5,",",Datos!C5,",",Datos!D5,",",Datos!E5,",",Datos!F5,",",Datos!G5,",",Datos!H5)</f>
@@ -681,13 +687,13 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E11" t="str">
         <f>CONCATENATE(Datos!A6,",",Datos!B6,",",Datos!C6,",",Datos!D6,",",Datos!E6,",",Datos!F6,",",Datos!G6,",",Datos!H6)</f>
@@ -696,13 +702,13 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E12" t="str">
         <f>CONCATENATE(Datos!A7,",",Datos!B7,",",Datos!C7,",",Datos!D7,",",Datos!E7,",",Datos!F7,",",Datos!G7,",",Datos!H7)</f>
@@ -711,13 +717,13 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D13" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E13" t="str">
         <f>CONCATENATE(Datos!A8,",",Datos!B8,",",Datos!C8,",",Datos!D8,",",Datos!E8,",",Datos!F8,",",Datos!G8,",",Datos!H8)</f>
@@ -726,13 +732,13 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D14" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E14" t="str">
         <f>CONCATENATE(Datos!A9,",",Datos!B9,",",Datos!C9,",",Datos!D9,",",Datos!E9,",",Datos!F9,",",Datos!G9,",",Datos!H9)</f>
@@ -741,13 +747,13 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D15" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E15" t="str">
         <f>CONCATENATE(Datos!A10,",",Datos!B10,",",Datos!C10,",",Datos!D10,",",Datos!E10,",",Datos!F10,",",Datos!G10,",",Datos!H10)</f>
@@ -755,225 +761,348 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" t="s">
+        <v>36</v>
+      </c>
       <c r="E16" t="str">
         <f>CONCATENATE(Datos!A11,",",Datos!B11,",",Datos!C11,",",Datos!D11,",",Datos!E11,",",Datos!F11,",",Datos!G11,",",Datos!H11)</f>
-        <v>access__for_group_name_,_for_,model_,group_name_,0,0,0,0</v>
+        <v>access_certifications_certification_for_group_name_certifications_ingenieria,certifications_certification_for_certifications_ingenieria,model_certifications_certification,group_name_certifications_ingenieria,1,1,1,1</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" t="s">
+        <v>36</v>
+      </c>
       <c r="E17" t="str">
         <f>CONCATENATE(Datos!A12,",",Datos!B12,",",Datos!C12,",",Datos!D12,",",Datos!E12,",",Datos!F12,",",Datos!G12,",",Datos!H12)</f>
-        <v>access__for_group_name_,_for_,model_,group_name_,0,0,0,0</v>
+        <v>access_certifications_certification_ceyf_for_group_name_certifications_ingenieria,certifications_certification_ceyf_for_certifications_ingenieria,model_certifications_certification_ceyf,group_name_certifications_ingenieria,1,1,1,1</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" t="s">
+        <v>36</v>
+      </c>
       <c r="E18" t="str">
         <f>CONCATENATE(Datos!A13,",",Datos!B13,",",Datos!C13,",",Datos!D13,",",Datos!E13,",",Datos!F13,",",Datos!G13,",",Datos!H13)</f>
-        <v>access__for_group_name_,_for_,model_,group_name_,0,0,0,0</v>
+        <v>access_certifications_certification_coiled_tubing_for_group_name_certifications_ingenieria,certifications_certification_coiled_tubing_for_certifications_ingenieria,model_certifications_certification_coiled_tubing,group_name_certifications_ingenieria,1,1,1,1</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" t="s">
+        <v>36</v>
+      </c>
       <c r="E19" t="str">
         <f>CONCATENATE(Datos!A14,",",Datos!B14,",",Datos!C14,",",Datos!D14,",",Datos!E14,",",Datos!F14,",",Datos!G14,",",Datos!H14)</f>
-        <v>access__for_group_name_,_for_,model_,group_name_,0,0,0,0</v>
+        <v>access_certifications_coiled_tubing_time_losed_for_group_name_certifications_ingenieria,certifications_coiled_tubing_time_losed_for_certifications_ingenieria,model_certifications_coiled_tubing_time_losed,group_name_certifications_ingenieria,1,1,1,1</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" t="s">
+        <v>36</v>
+      </c>
       <c r="E20" t="str">
         <f>CONCATENATE(Datos!A15,",",Datos!B15,",",Datos!C15,",",Datos!D15,",",Datos!E15,",",Datos!F15,",",Datos!G15,",",Datos!H15)</f>
-        <v>access__for_group_name_,_for_,model_,group_name_,0,0,0,0</v>
+        <v>access_certifications_certification_task_for_group_name_certifications_ingenieria,certifications_certification_task_for_certifications_ingenieria,model_certifications_certification_task,group_name_certifications_ingenieria,1,1,1,1</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" t="s">
+        <v>36</v>
+      </c>
       <c r="E21" t="str">
         <f>CONCATENATE(Datos!A16,",",Datos!B16,",",Datos!C16,",",Datos!D16,",",Datos!E16,",",Datos!F16,",",Datos!G16,",",Datos!H16)</f>
-        <v>access__for_group_name_,_for_,model_,group_name_,0,0,0,0</v>
+        <v>access_certifications_certification_task_stage_for_group_name_certifications_ingenieria,certifications_certification_task_stage_for_certifications_ingenieria,model_certifications_certification_task_stage,group_name_certifications_ingenieria,1,1,1,1</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" t="s">
+        <v>36</v>
+      </c>
       <c r="E22" t="str">
         <f>CONCATENATE(Datos!A17,",",Datos!B17,",",Datos!C17,",",Datos!D17,",",Datos!E17,",",Datos!F17,",",Datos!G17,",",Datos!H17)</f>
-        <v>access__for_group_name_,_for_,model_,group_name_,0,0,0,0</v>
+        <v>access_certification_invoice_for_group_name_certifications_ingenieria,certification_invoice_for_certifications_ingenieria,model_certification_invoice,group_name_certifications_ingenieria,1,1,1,1</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" t="s">
+        <v>36</v>
+      </c>
       <c r="E23" t="str">
         <f>CONCATENATE(Datos!A18,",",Datos!B18,",",Datos!C18,",",Datos!D18,",",Datos!E18,",",Datos!F18,",",Datos!G18,",",Datos!H18)</f>
-        <v>access__for_group_name_,_for_,model_,group_name_,0,0,0,0</v>
+        <v>access_certifications_supervisor_for_group_name_certifications_ingenieria,certifications_supervisor_for_certifications_ingenieria,model_certifications_supervisor,group_name_certifications_ingenieria,1,1,1,1</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" t="s">
+        <v>36</v>
+      </c>
       <c r="E24" t="str">
         <f>CONCATENATE(Datos!A19,",",Datos!B19,",",Datos!C19,",",Datos!D19,",",Datos!E19,",",Datos!F19,",",Datos!G19,",",Datos!H19)</f>
-        <v>access__for_group_name_,_for_,model_,group_name_,0,0,0,0</v>
+        <v>access_certification_contract_for_group_name_certifications_ingenieria,certification_contract_for_certifications_ingenieria,model_certification_contract,group_name_certifications_ingenieria,1,1,1,1</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" t="s">
+        <v>37</v>
+      </c>
       <c r="E25" t="str">
         <f>CONCATENATE(Datos!A20,",",Datos!B20,",",Datos!C20,",",Datos!D20,",",Datos!E20,",",Datos!F20,",",Datos!G20,",",Datos!H20)</f>
-        <v>access__for_group_name_,_for_,model_,group_name_,0,0,0,0</v>
+        <v>access_certifications_certification_for_group_name_certifications_administracion,certifications_certification_for_certifications_administracion,model_certifications_certification,group_name_certifications_administracion,1,1,1,1</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C26" t="s">
-        <v>3</v>
+        <v>39</v>
+      </c>
+      <c r="D26" t="s">
+        <v>37</v>
       </c>
       <c r="E26" t="str">
         <f>CONCATENATE(Datos!A21,",",Datos!B21,",",Datos!C21,",",Datos!D21,",",Datos!E21,",",Datos!F21,",",Datos!G21,",",Datos!H21)</f>
-        <v>access_vehicle_model_for_group_name_,vehicle_model_for_,model_vehicle_model,group_name_,1,0,0,0</v>
+        <v>access_certifications_certification_ceyf_for_group_name_certifications_administracion,certifications_certification_ceyf_for_certifications_administracion,model_certifications_certification_ceyf,group_name_certifications_administracion,1,1,0,0</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C27" t="s">
-        <v>3</v>
+        <v>39</v>
+      </c>
+      <c r="D27" t="s">
+        <v>37</v>
       </c>
       <c r="E27" t="str">
         <f>CONCATENATE(Datos!A22,",",Datos!B22,",",Datos!C22,",",Datos!D22,",",Datos!E22,",",Datos!F22,",",Datos!G22,",",Datos!H22)</f>
-        <v>access_vehicle_color_for_group_name_,vehicle_color_for_,model_vehicle_color,group_name_,1,0,0,0</v>
+        <v>access_certifications_certification_coiled_tubing_for_group_name_certifications_administracion,certifications_certification_coiled_tubing_for_certifications_administracion,model_certifications_certification_coiled_tubing,group_name_certifications_administracion,1,1,0,0</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>3</v>
+        <v>38</v>
+      </c>
+      <c r="D28" t="s">
+        <v>37</v>
       </c>
       <c r="E28" t="str">
         <f>CONCATENATE(Datos!A23,",",Datos!B23,",",Datos!C23,",",Datos!D23,",",Datos!E23,",",Datos!F23,",",Datos!G23,",",Datos!H23)</f>
-        <v>access_vehicle_status_for_group_name_,vehicle_status_for_,model_vehicle_status,group_name_,1,0,0,0</v>
+        <v>access_certifications_coiled_tubing_time_losed_for_group_name_certifications_administracion,certifications_coiled_tubing_time_losed_for_certifications_administracion,model_certifications_coiled_tubing_time_losed,group_name_certifications_administracion,1,0,0,0</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="C29" t="s">
-        <v>3</v>
+        <v>15</v>
+      </c>
+      <c r="D29" t="s">
+        <v>37</v>
       </c>
       <c r="E29" t="str">
         <f>CONCATENATE(Datos!A24,",",Datos!B24,",",Datos!C24,",",Datos!D24,",",Datos!E24,",",Datos!F24,",",Datos!G24,",",Datos!H24)</f>
-        <v>access_res_partner_for_group_name_,res_partner_for_,model_res_partner,group_name_,1,0,0,0</v>
+        <v>access_certifications_certification_task_for_group_name_certifications_administracion,certifications_certification_task_for_certifications_administracion,model_certifications_certification_task,group_name_certifications_administracion,1,1,1,1</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C30" t="s">
-        <v>3</v>
+        <v>15</v>
+      </c>
+      <c r="D30" t="s">
+        <v>37</v>
       </c>
       <c r="E30" t="str">
         <f>CONCATENATE(Datos!A25,",",Datos!B25,",",Datos!C25,",",Datos!D25,",",Datos!E25,",",Datos!F25,",",Datos!G25,",",Datos!H25)</f>
-        <v>access_config_for_group_name_,config_for_,model_config,group_name_,1,0,0,0</v>
+        <v>access_certifications_certification_task_stage_for_group_name_certifications_administracion,certifications_certification_task_stage_for_certifications_administracion,model_certifications_certification_task_stage,group_name_certifications_administracion,1,1,1,1</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="C31" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="D31" t="s">
+        <v>37</v>
       </c>
       <c r="E31" t="str">
         <f>CONCATENATE(Datos!A26,",",Datos!B26,",",Datos!C26,",",Datos!D26,",",Datos!E26,",",Datos!F26,",",Datos!G26,",",Datos!H26)</f>
-        <v>access_vehicle_for_group_name_,vehicle_for_,model_vehicle,group_name_,1,1,1,1</v>
+        <v>access_certification_invoice_for_group_name_certifications_administracion,certification_invoice_for_certifications_administracion,model_certification_invoice,group_name_certifications_administracion,1,1,1,1</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="C32" t="s">
-        <v>16</v>
+        <v>38</v>
+      </c>
+      <c r="D32" t="s">
+        <v>37</v>
       </c>
       <c r="E32" t="str">
         <f>CONCATENATE(Datos!A27,",",Datos!B27,",",Datos!C27,",",Datos!D27,",",Datos!E27,",",Datos!F27,",",Datos!G27,",",Datos!H27)</f>
-        <v>access_vehicle_model_for_group_name_,vehicle_model_for_,model_vehicle_model,group_name_,1,1,1,1</v>
+        <v>access_certifications_supervisor_for_group_name_certifications_administracion,certifications_supervisor_for_certifications_administracion,model_certifications_supervisor,group_name_certifications_administracion,1,0,0,0</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C33" t="s">
-        <v>16</v>
+        <v>38</v>
+      </c>
+      <c r="D33" t="s">
+        <v>37</v>
       </c>
       <c r="E33" t="str">
         <f>CONCATENATE(Datos!A28,",",Datos!B28,",",Datos!C28,",",Datos!D28,",",Datos!E28,",",Datos!F28,",",Datos!G28,",",Datos!H28)</f>
-        <v>access_config_for_group_name_,config_for_,model_vehicle_color,group_name_,1,1,1,1</v>
+        <v>access_certification_contract_for_group_name_certifications_administracion,certification_contract_for_certifications_administracion,model_certification_contract,group_name_certifications_administracion,1,0,0,0</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="C34" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="D34" t="s">
+        <v>41</v>
       </c>
       <c r="E34" t="str">
         <f>CONCATENATE(Datos!A29,",",Datos!B29,",",Datos!C29,",",Datos!D29,",",Datos!E29,",",Datos!F29,",",Datos!G29,",",Datos!H29)</f>
-        <v>access_vehicle_for_group_name_,vehicle_for_,model_vehicle_status,group_name_,1,1,1,1</v>
+        <v>access_exchange_cotizacion_dolar_bcra_for_group_name_exchange_administrator,exchange_cotizacion_dolar_bcra_for_exchange_administrator,model_exchange_cotizacion_dolar_bcra,group_name_exchange_administrator,1,1,1,1</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="C35" t="s">
-        <v>16</v>
+        <v>38</v>
+      </c>
+      <c r="D35" t="s">
+        <v>43</v>
       </c>
       <c r="E35" t="str">
         <f>CONCATENATE(Datos!A30,",",Datos!B30,",",Datos!C30,",",Datos!D30,",",Datos!E30,",",Datos!F30,",",Datos!G30,",",Datos!H30)</f>
-        <v>access_vehicle_model_for_group_name_,vehicle_model_for_,model_res_partner,group_name_,1,1,1,1</v>
+        <v>access_exchange_cotizacion_dolar_bcra_for_group_name_solo_lectura,exchange_cotizacion_dolar_bcra_for_solo_lectura,model_exchange_cotizacion_dolar_bcra,group_name_solo_lectura,1,0,0,0</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="C36" t="s">
-        <v>16</v>
+        <v>40</v>
+      </c>
+      <c r="D36" t="s">
+        <v>42</v>
       </c>
       <c r="E36" t="str">
         <f>CONCATENATE(Datos!A31,",",Datos!B31,",",Datos!C31,",",Datos!D31,",",Datos!E31,",",Datos!F31,",",Datos!G31,",",Datos!H31)</f>
-        <v>access_vehicle_color_for_group_name_,vehicle_color_for_,model_config,group_name_,1,1,1,1</v>
+        <v>access_exchange_cotizacion_dolar_bcra_for_group_name_exchange_administracion,exchange_cotizacion_dolar_bcra_for_exchange_administracion,model_exchange_cotizacion_dolar_bcra,group_name_exchange_administracion,1,1,1,0</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E37" t="str">
         <f>CONCATENATE(Datos!A32,",",Datos!B32,",",Datos!C32,",",Datos!D32,",",Datos!E32,",",Datos!F32,",",Datos!G32,",",Datos!H32)</f>
-        <v>access_vehicle_status_for_group_name_,vehicle_status_for_,model_,group_name_,0,0,0,0</v>
+        <v>access__for_group_name_,_for_,model_,group_name_,0,0,0,0</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E38" t="str">
         <f>CONCATENATE(Datos!A33,",",Datos!B33,",",Datos!C33,",",Datos!D33,",",Datos!E33,",",Datos!F33,",",Datos!G33,",",Datos!H33)</f>
-        <v>access__for_group_name_,_for_,model_,group_name_,0,0,0,0</v>
+        <v>access_exchange_cotizacion_dolar_bcra_for_group_name_,_for_,model_,group_name_,0,0,0,0</v>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E39" t="str">
         <f>CONCATENATE(Datos!A34,",",Datos!B34,",",Datos!C34,",",Datos!D34,",",Datos!E34,",",Datos!F34,",",Datos!G34,",",Datos!H34)</f>
-        <v>access__for_group_name_,_for_,model_,group_name_,0,0,0,0</v>
+        <v>access_exchange_cotizacion_dolar_bcra_for_group_name_,_for_,model_,group_name_,0,0,0,0</v>
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E40" t="str">
         <f>CONCATENATE(Datos!A35,",",Datos!B35,",",Datos!C35,",",Datos!D35,",",Datos!E35,",",Datos!F35,",",Datos!G35,",",Datos!H35)</f>
-        <v>access_res_partner_for_group_name_,res_partner_for_,model_,group_name_,0,0,0,0</v>
+        <v>access__for_group_name_,exchange_cotizacion_dolar_bcra_for_,model_,group_name_,0,0,0,0</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E41" t="str">
         <f>CONCATENATE(Datos!A36,",",Datos!B36,",",Datos!C36,",",Datos!D36,",",Datos!E36,",",Datos!F36,",",Datos!G36,",",Datos!H36)</f>
-        <v>access_config_for_group_name_,config_for_,model_,group_name_,0,0,0,0</v>
+        <v>access__for_group_name_,exchange_cotizacion_dolar_bcra_for_,model_,group_name_,0,0,0,0</v>
       </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
@@ -1064,13 +1193,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21:D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="58.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="88.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="33.42578125" customWidth="1"/>
     <col min="4" max="4" width="36.28515625" customWidth="1"/>
     <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
@@ -1079,28 +1208,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>10</v>
-      </c>
-      <c r="H1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1412,359 +1541,359 @@
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>CONCATENATE("access_",Permisos!B16,"_for_","group_name_",Permisos!D16)</f>
-        <v>access__for_group_name_</v>
+        <v>access_certifications_certification_for_group_name_certifications_ingenieria</v>
       </c>
       <c r="B11" t="str">
         <f>CONCATENATE(Permisos!B16,"_for_",Permisos!D16)</f>
-        <v>_for_</v>
+        <v>certifications_certification_for_certifications_ingenieria</v>
       </c>
       <c r="C11" t="str">
         <f>CONCATENATE("model_",Permisos!B16)</f>
-        <v>model_</v>
+        <v>model_certifications_certification</v>
       </c>
       <c r="D11" t="str">
         <f>CONCATENATE("group_name_",Permisos!D16)</f>
-        <v>group_name_</v>
+        <v>group_name_certifications_ingenieria</v>
       </c>
       <c r="E11" t="str">
         <f>IF(ISNUMBER(SEARCH("read",Permisos!$C16)),"1","0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" t="str">
         <f>IF(ISNUMBER(SEARCH("write",Permisos!$C16)),"1","0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11" t="str">
         <f>IF(ISNUMBER(SEARCH("create",Permisos!$C16)),"1","0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" t="str">
         <f>IF(ISNUMBER(SEARCH("unlink",Permisos!$C16)),"1","0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f>CONCATENATE("access_",Permisos!B17,"_for_","group_name_",Permisos!D17)</f>
-        <v>access__for_group_name_</v>
+        <v>access_certifications_certification_ceyf_for_group_name_certifications_ingenieria</v>
       </c>
       <c r="B12" t="str">
         <f>CONCATENATE(Permisos!B17,"_for_",Permisos!D17)</f>
-        <v>_for_</v>
+        <v>certifications_certification_ceyf_for_certifications_ingenieria</v>
       </c>
       <c r="C12" t="str">
         <f>CONCATENATE("model_",Permisos!B17)</f>
-        <v>model_</v>
+        <v>model_certifications_certification_ceyf</v>
       </c>
       <c r="D12" t="str">
         <f>CONCATENATE("group_name_",Permisos!D17)</f>
-        <v>group_name_</v>
+        <v>group_name_certifications_ingenieria</v>
       </c>
       <c r="E12" t="str">
         <f>IF(ISNUMBER(SEARCH("read",Permisos!$C17)),"1","0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" t="str">
         <f>IF(ISNUMBER(SEARCH("write",Permisos!$C17)),"1","0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" t="str">
         <f>IF(ISNUMBER(SEARCH("create",Permisos!$C17)),"1","0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" t="str">
         <f>IF(ISNUMBER(SEARCH("unlink",Permisos!$C17)),"1","0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f>CONCATENATE("access_",Permisos!B18,"_for_","group_name_",Permisos!D18)</f>
-        <v>access__for_group_name_</v>
+        <v>access_certifications_certification_coiled_tubing_for_group_name_certifications_ingenieria</v>
       </c>
       <c r="B13" t="str">
         <f>CONCATENATE(Permisos!B18,"_for_",Permisos!D18)</f>
-        <v>_for_</v>
+        <v>certifications_certification_coiled_tubing_for_certifications_ingenieria</v>
       </c>
       <c r="C13" t="str">
         <f>CONCATENATE("model_",Permisos!B18)</f>
-        <v>model_</v>
+        <v>model_certifications_certification_coiled_tubing</v>
       </c>
       <c r="D13" t="str">
         <f>CONCATENATE("group_name_",Permisos!D18)</f>
-        <v>group_name_</v>
+        <v>group_name_certifications_ingenieria</v>
       </c>
       <c r="E13" t="str">
         <f>IF(ISNUMBER(SEARCH("read",Permisos!$C18)),"1","0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" t="str">
         <f>IF(ISNUMBER(SEARCH("write",Permisos!$C18)),"1","0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" t="str">
         <f>IF(ISNUMBER(SEARCH("create",Permisos!$C18)),"1","0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" t="str">
         <f>IF(ISNUMBER(SEARCH("unlink",Permisos!$C18)),"1","0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f>CONCATENATE("access_",Permisos!B19,"_for_","group_name_",Permisos!D19)</f>
-        <v>access__for_group_name_</v>
+        <v>access_certifications_coiled_tubing_time_losed_for_group_name_certifications_ingenieria</v>
       </c>
       <c r="B14" t="str">
         <f>CONCATENATE(Permisos!B19,"_for_",Permisos!D19)</f>
-        <v>_for_</v>
+        <v>certifications_coiled_tubing_time_losed_for_certifications_ingenieria</v>
       </c>
       <c r="C14" t="str">
         <f>CONCATENATE("model_",Permisos!B19)</f>
-        <v>model_</v>
+        <v>model_certifications_coiled_tubing_time_losed</v>
       </c>
       <c r="D14" t="str">
         <f>CONCATENATE("group_name_",Permisos!D19)</f>
-        <v>group_name_</v>
+        <v>group_name_certifications_ingenieria</v>
       </c>
       <c r="E14" t="str">
         <f>IF(ISNUMBER(SEARCH("read",Permisos!$C19)),"1","0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" t="str">
         <f>IF(ISNUMBER(SEARCH("write",Permisos!$C19)),"1","0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" t="str">
         <f>IF(ISNUMBER(SEARCH("create",Permisos!$C19)),"1","0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" t="str">
         <f>IF(ISNUMBER(SEARCH("unlink",Permisos!$C19)),"1","0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f>CONCATENATE("access_",Permisos!B20,"_for_","group_name_",Permisos!D20)</f>
-        <v>access__for_group_name_</v>
+        <v>access_certifications_certification_task_for_group_name_certifications_ingenieria</v>
       </c>
       <c r="B15" t="str">
         <f>CONCATENATE(Permisos!B20,"_for_",Permisos!D20)</f>
-        <v>_for_</v>
+        <v>certifications_certification_task_for_certifications_ingenieria</v>
       </c>
       <c r="C15" t="str">
         <f>CONCATENATE("model_",Permisos!B20)</f>
-        <v>model_</v>
+        <v>model_certifications_certification_task</v>
       </c>
       <c r="D15" t="str">
         <f>CONCATENATE("group_name_",Permisos!D20)</f>
-        <v>group_name_</v>
+        <v>group_name_certifications_ingenieria</v>
       </c>
       <c r="E15" t="str">
         <f>IF(ISNUMBER(SEARCH("read",Permisos!$C20)),"1","0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" t="str">
         <f>IF(ISNUMBER(SEARCH("write",Permisos!$C20)),"1","0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15" t="str">
         <f>IF(ISNUMBER(SEARCH("create",Permisos!$C20)),"1","0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" t="str">
         <f>IF(ISNUMBER(SEARCH("unlink",Permisos!$C20)),"1","0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f>CONCATENATE("access_",Permisos!B21,"_for_","group_name_",Permisos!D21)</f>
-        <v>access__for_group_name_</v>
+        <v>access_certifications_certification_task_stage_for_group_name_certifications_ingenieria</v>
       </c>
       <c r="B16" t="str">
         <f>CONCATENATE(Permisos!B21,"_for_",Permisos!D21)</f>
-        <v>_for_</v>
+        <v>certifications_certification_task_stage_for_certifications_ingenieria</v>
       </c>
       <c r="C16" t="str">
         <f>CONCATENATE("model_",Permisos!B21)</f>
-        <v>model_</v>
+        <v>model_certifications_certification_task_stage</v>
       </c>
       <c r="D16" t="str">
         <f>CONCATENATE("group_name_",Permisos!D21)</f>
-        <v>group_name_</v>
+        <v>group_name_certifications_ingenieria</v>
       </c>
       <c r="E16" t="str">
         <f>IF(ISNUMBER(SEARCH("read",Permisos!$C21)),"1","0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" t="str">
         <f>IF(ISNUMBER(SEARCH("write",Permisos!$C21)),"1","0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16" t="str">
         <f>IF(ISNUMBER(SEARCH("create",Permisos!$C21)),"1","0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" t="str">
         <f>IF(ISNUMBER(SEARCH("unlink",Permisos!$C21)),"1","0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f>CONCATENATE("access_",Permisos!B22,"_for_","group_name_",Permisos!D22)</f>
-        <v>access__for_group_name_</v>
+        <v>access_certification_invoice_for_group_name_certifications_ingenieria</v>
       </c>
       <c r="B17" t="str">
         <f>CONCATENATE(Permisos!B22,"_for_",Permisos!D22)</f>
-        <v>_for_</v>
+        <v>certification_invoice_for_certifications_ingenieria</v>
       </c>
       <c r="C17" t="str">
         <f>CONCATENATE("model_",Permisos!B22)</f>
-        <v>model_</v>
+        <v>model_certification_invoice</v>
       </c>
       <c r="D17" t="str">
         <f>CONCATENATE("group_name_",Permisos!D22)</f>
-        <v>group_name_</v>
+        <v>group_name_certifications_ingenieria</v>
       </c>
       <c r="E17" t="str">
         <f>IF(ISNUMBER(SEARCH("read",Permisos!$C22)),"1","0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" t="str">
         <f>IF(ISNUMBER(SEARCH("write",Permisos!$C22)),"1","0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17" t="str">
         <f>IF(ISNUMBER(SEARCH("create",Permisos!$C22)),"1","0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" t="str">
         <f>IF(ISNUMBER(SEARCH("unlink",Permisos!$C22)),"1","0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f>CONCATENATE("access_",Permisos!B23,"_for_","group_name_",Permisos!D23)</f>
-        <v>access__for_group_name_</v>
+        <v>access_certifications_supervisor_for_group_name_certifications_ingenieria</v>
       </c>
       <c r="B18" t="str">
         <f>CONCATENATE(Permisos!B23,"_for_",Permisos!D23)</f>
-        <v>_for_</v>
+        <v>certifications_supervisor_for_certifications_ingenieria</v>
       </c>
       <c r="C18" t="str">
         <f>CONCATENATE("model_",Permisos!B23)</f>
-        <v>model_</v>
+        <v>model_certifications_supervisor</v>
       </c>
       <c r="D18" t="str">
         <f>CONCATENATE("group_name_",Permisos!D23)</f>
-        <v>group_name_</v>
+        <v>group_name_certifications_ingenieria</v>
       </c>
       <c r="E18" t="str">
         <f>IF(ISNUMBER(SEARCH("read",Permisos!$C23)),"1","0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18" t="str">
         <f>IF(ISNUMBER(SEARCH("write",Permisos!$C23)),"1","0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18" t="str">
         <f>IF(ISNUMBER(SEARCH("create",Permisos!$C23)),"1","0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18" t="str">
         <f>IF(ISNUMBER(SEARCH("unlink",Permisos!$C23)),"1","0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f>CONCATENATE("access_",Permisos!B24,"_for_","group_name_",Permisos!D24)</f>
-        <v>access__for_group_name_</v>
+        <v>access_certification_contract_for_group_name_certifications_ingenieria</v>
       </c>
       <c r="B19" t="str">
         <f>CONCATENATE(Permisos!B24,"_for_",Permisos!D24)</f>
-        <v>_for_</v>
+        <v>certification_contract_for_certifications_ingenieria</v>
       </c>
       <c r="C19" t="str">
         <f>CONCATENATE("model_",Permisos!B24)</f>
-        <v>model_</v>
+        <v>model_certification_contract</v>
       </c>
       <c r="D19" t="str">
         <f>CONCATENATE("group_name_",Permisos!D24)</f>
-        <v>group_name_</v>
+        <v>group_name_certifications_ingenieria</v>
       </c>
       <c r="E19" t="str">
         <f>IF(ISNUMBER(SEARCH("read",Permisos!$C24)),"1","0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19" t="str">
         <f>IF(ISNUMBER(SEARCH("write",Permisos!$C24)),"1","0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19" t="str">
         <f>IF(ISNUMBER(SEARCH("create",Permisos!$C24)),"1","0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19" t="str">
         <f>IF(ISNUMBER(SEARCH("unlink",Permisos!$C24)),"1","0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f>CONCATENATE("access_",Permisos!B25,"_for_","group_name_",Permisos!D25)</f>
-        <v>access__for_group_name_</v>
+        <v>access_certifications_certification_for_group_name_certifications_administracion</v>
       </c>
       <c r="B20" t="str">
         <f>CONCATENATE(Permisos!B25,"_for_",Permisos!D25)</f>
-        <v>_for_</v>
+        <v>certifications_certification_for_certifications_administracion</v>
       </c>
       <c r="C20" t="str">
         <f>CONCATENATE("model_",Permisos!B25)</f>
-        <v>model_</v>
+        <v>model_certifications_certification</v>
       </c>
       <c r="D20" t="str">
         <f>CONCATENATE("group_name_",Permisos!D25)</f>
-        <v>group_name_</v>
+        <v>group_name_certifications_administracion</v>
       </c>
       <c r="E20" t="str">
         <f>IF(ISNUMBER(SEARCH("read",Permisos!$C25)),"1","0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20" t="str">
         <f>IF(ISNUMBER(SEARCH("write",Permisos!$C25)),"1","0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20" t="str">
         <f>IF(ISNUMBER(SEARCH("create",Permisos!$C25)),"1","0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20" t="str">
         <f>IF(ISNUMBER(SEARCH("unlink",Permisos!$C25)),"1","0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f>CONCATENATE("access_",Permisos!B26,"_for_","group_name_",Permisos!D26)</f>
-        <v>access_vehicle_model_for_group_name_</v>
+        <v>access_certifications_certification_ceyf_for_group_name_certifications_administracion</v>
       </c>
       <c r="B21" t="str">
         <f>CONCATENATE(Permisos!B26,"_for_",Permisos!D26)</f>
-        <v>vehicle_model_for_</v>
+        <v>certifications_certification_ceyf_for_certifications_administracion</v>
       </c>
       <c r="C21" t="str">
         <f>CONCATENATE("model_",Permisos!B26)</f>
-        <v>model_vehicle_model</v>
+        <v>model_certifications_certification_ceyf</v>
       </c>
       <c r="D21" t="str">
         <f>CONCATENATE("group_name_",Permisos!D26)</f>
-        <v>group_name_</v>
+        <v>group_name_certifications_administracion</v>
       </c>
       <c r="E21" t="str">
         <f>IF(ISNUMBER(SEARCH("read",Permisos!$C26)),"1","0")</f>
@@ -1772,7 +1901,7 @@
       </c>
       <c r="F21" t="str">
         <f>IF(ISNUMBER(SEARCH("write",Permisos!$C26)),"1","0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G21" t="str">
         <f>IF(ISNUMBER(SEARCH("create",Permisos!$C26)),"1","0")</f>
@@ -1786,19 +1915,19 @@
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f>CONCATENATE("access_",Permisos!B27,"_for_","group_name_",Permisos!D27)</f>
-        <v>access_vehicle_color_for_group_name_</v>
+        <v>access_certifications_certification_coiled_tubing_for_group_name_certifications_administracion</v>
       </c>
       <c r="B22" t="str">
         <f>CONCATENATE(Permisos!B27,"_for_",Permisos!D27)</f>
-        <v>vehicle_color_for_</v>
+        <v>certifications_certification_coiled_tubing_for_certifications_administracion</v>
       </c>
       <c r="C22" t="str">
         <f>CONCATENATE("model_",Permisos!B27)</f>
-        <v>model_vehicle_color</v>
+        <v>model_certifications_certification_coiled_tubing</v>
       </c>
       <c r="D22" t="str">
         <f>CONCATENATE("group_name_",Permisos!D27)</f>
-        <v>group_name_</v>
+        <v>group_name_certifications_administracion</v>
       </c>
       <c r="E22" t="str">
         <f>IF(ISNUMBER(SEARCH("read",Permisos!$C27)),"1","0")</f>
@@ -1806,7 +1935,7 @@
       </c>
       <c r="F22" t="str">
         <f>IF(ISNUMBER(SEARCH("write",Permisos!$C27)),"1","0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22" t="str">
         <f>IF(ISNUMBER(SEARCH("create",Permisos!$C27)),"1","0")</f>
@@ -1820,19 +1949,19 @@
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f>CONCATENATE("access_",Permisos!B28,"_for_","group_name_",Permisos!D28)</f>
-        <v>access_vehicle_status_for_group_name_</v>
+        <v>access_certifications_coiled_tubing_time_losed_for_group_name_certifications_administracion</v>
       </c>
       <c r="B23" t="str">
         <f>CONCATENATE(Permisos!B28,"_for_",Permisos!D28)</f>
-        <v>vehicle_status_for_</v>
+        <v>certifications_coiled_tubing_time_losed_for_certifications_administracion</v>
       </c>
       <c r="C23" t="str">
         <f>CONCATENATE("model_",Permisos!B28)</f>
-        <v>model_vehicle_status</v>
+        <v>model_certifications_coiled_tubing_time_losed</v>
       </c>
       <c r="D23" t="str">
         <f>CONCATENATE("group_name_",Permisos!D28)</f>
-        <v>group_name_</v>
+        <v>group_name_certifications_administracion</v>
       </c>
       <c r="E23" t="str">
         <f>IF(ISNUMBER(SEARCH("read",Permisos!$C28)),"1","0")</f>
@@ -1853,20 +1982,20 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
-        <f>CONCATENATE("access_",Permisos!B29,"_for_","group_name_",Permisos!D27)</f>
-        <v>access_res_partner_for_group_name_</v>
+        <f>CONCATENATE("access_",Permisos!B29,"_for_","group_name_",Permisos!D29)</f>
+        <v>access_certifications_certification_task_for_group_name_certifications_administracion</v>
       </c>
       <c r="B24" t="str">
-        <f>CONCATENATE(Permisos!B29,"_for_",Permisos!D27)</f>
-        <v>res_partner_for_</v>
+        <f>CONCATENATE(Permisos!B29,"_for_",Permisos!D29)</f>
+        <v>certifications_certification_task_for_certifications_administracion</v>
       </c>
       <c r="C24" t="str">
         <f>CONCATENATE("model_",Permisos!B29)</f>
-        <v>model_res_partner</v>
+        <v>model_certifications_certification_task</v>
       </c>
       <c r="D24" t="str">
         <f>CONCATENATE("group_name_",Permisos!D29)</f>
-        <v>group_name_</v>
+        <v>group_name_certifications_administracion</v>
       </c>
       <c r="E24" t="str">
         <f>IF(ISNUMBER(SEARCH("read",Permisos!$C29)),"1","0")</f>
@@ -1874,33 +2003,33 @@
       </c>
       <c r="F24" t="str">
         <f>IF(ISNUMBER(SEARCH("write",Permisos!$C29)),"1","0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24" t="str">
         <f>IF(ISNUMBER(SEARCH("create",Permisos!$C29)),"1","0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24" t="str">
         <f>IF(ISNUMBER(SEARCH("unlink",Permisos!$C29)),"1","0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
-        <f>CONCATENATE("access_",Permisos!B30,"_for_","group_name_",Permisos!D28)</f>
-        <v>access_config_for_group_name_</v>
+        <f>CONCATENATE("access_",Permisos!B30,"_for_","group_name_",Permisos!D30)</f>
+        <v>access_certifications_certification_task_stage_for_group_name_certifications_administracion</v>
       </c>
       <c r="B25" t="str">
-        <f>CONCATENATE(Permisos!B30,"_for_",Permisos!D28)</f>
-        <v>config_for_</v>
+        <f>CONCATENATE(Permisos!B30,"_for_",Permisos!D30)</f>
+        <v>certifications_certification_task_stage_for_certifications_administracion</v>
       </c>
       <c r="C25" t="str">
         <f>CONCATENATE("model_",Permisos!B30)</f>
-        <v>model_config</v>
+        <v>model_certifications_certification_task_stage</v>
       </c>
       <c r="D25" t="str">
         <f>CONCATENATE("group_name_",Permisos!D30)</f>
-        <v>group_name_</v>
+        <v>group_name_certifications_administracion</v>
       </c>
       <c r="E25" t="str">
         <f>IF(ISNUMBER(SEARCH("read",Permisos!$C30)),"1","0")</f>
@@ -1908,33 +2037,33 @@
       </c>
       <c r="F25" t="str">
         <f>IF(ISNUMBER(SEARCH("write",Permisos!$C30)),"1","0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25" t="str">
         <f>IF(ISNUMBER(SEARCH("create",Permisos!$C30)),"1","0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H25" t="str">
         <f>IF(ISNUMBER(SEARCH("unlink",Permisos!$C30)),"1","0")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
-        <f>CONCATENATE("access_",Permisos!B31,"_for_","group_name_",Permisos!D29)</f>
-        <v>access_vehicle_for_group_name_</v>
+        <f>CONCATENATE("access_",Permisos!B31,"_for_","group_name_",Permisos!D31)</f>
+        <v>access_certification_invoice_for_group_name_certifications_administracion</v>
       </c>
       <c r="B26" t="str">
-        <f>CONCATENATE(Permisos!B31,"_for_",Permisos!D29)</f>
-        <v>vehicle_for_</v>
+        <f>CONCATENATE(Permisos!B31,"_for_",Permisos!D31)</f>
+        <v>certification_invoice_for_certifications_administracion</v>
       </c>
       <c r="C26" t="str">
         <f>CONCATENATE("model_",Permisos!B31)</f>
-        <v>model_vehicle</v>
+        <v>model_certification_invoice</v>
       </c>
       <c r="D26" t="str">
         <f>CONCATENATE("group_name_",Permisos!D31)</f>
-        <v>group_name_</v>
+        <v>group_name_certifications_administracion</v>
       </c>
       <c r="E26" t="str">
         <f>IF(ISNUMBER(SEARCH("read",Permisos!$C31)),"1","0")</f>
@@ -1955,20 +2084,20 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
-        <f>CONCATENATE("access_",Permisos!B32,"_for_","group_name_",Permisos!D30)</f>
-        <v>access_vehicle_model_for_group_name_</v>
+        <f>CONCATENATE("access_",Permisos!B32,"_for_","group_name_",Permisos!D32)</f>
+        <v>access_certifications_supervisor_for_group_name_certifications_administracion</v>
       </c>
       <c r="B27" t="str">
-        <f>CONCATENATE(Permisos!B32,"_for_",Permisos!D30)</f>
-        <v>vehicle_model_for_</v>
+        <f>CONCATENATE(Permisos!B32,"_for_",Permisos!D32)</f>
+        <v>certifications_supervisor_for_certifications_administracion</v>
       </c>
       <c r="C27" t="str">
         <f>CONCATENATE("model_",Permisos!B32)</f>
-        <v>model_vehicle_model</v>
+        <v>model_certifications_supervisor</v>
       </c>
       <c r="D27" t="str">
-        <f>CONCATENATE("group_name_",Permisos!D30)</f>
-        <v>group_name_</v>
+        <f>CONCATENATE("group_name_",Permisos!D32)</f>
+        <v>group_name_certifications_administracion</v>
       </c>
       <c r="E27" t="str">
         <f>IF(ISNUMBER(SEARCH("read",Permisos!$C32)),"1","0")</f>
@@ -1976,33 +2105,33 @@
       </c>
       <c r="F27" t="str">
         <f>IF(ISNUMBER(SEARCH("write",Permisos!$C32)),"1","0")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G27" t="str">
         <f>IF(ISNUMBER(SEARCH("create",Permisos!$C32)),"1","0")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H27" t="str">
         <f>IF(ISNUMBER(SEARCH("unlink",Permisos!$C32)),"1","0")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
-        <f>CONCATENATE("access_",Permisos!B30,"_for_","group_name_",Permisos!D32)</f>
-        <v>access_config_for_group_name_</v>
+        <f>CONCATENATE("access_",Permisos!B33,"_for_","group_name_",Permisos!D33)</f>
+        <v>access_certification_contract_for_group_name_certifications_administracion</v>
       </c>
       <c r="B28" t="str">
-        <f>CONCATENATE(Permisos!B30,"_for_",Permisos!D32)</f>
-        <v>config_for_</v>
+        <f>CONCATENATE(Permisos!B33,"_for_",Permisos!D33)</f>
+        <v>certification_contract_for_certifications_administracion</v>
       </c>
       <c r="C28" t="str">
         <f>CONCATENATE("model_",Permisos!B33)</f>
-        <v>model_vehicle_color</v>
+        <v>model_certification_contract</v>
       </c>
       <c r="D28" t="str">
-        <f>CONCATENATE("group_name_",Permisos!D32)</f>
-        <v>group_name_</v>
+        <f>CONCATENATE("group_name_",Permisos!D33)</f>
+        <v>group_name_certifications_administracion</v>
       </c>
       <c r="E28" t="str">
         <f>IF(ISNUMBER(SEARCH("read",Permisos!$C33)),"1","0")</f>
@@ -2010,33 +2139,33 @@
       </c>
       <c r="F28" t="str">
         <f>IF(ISNUMBER(SEARCH("write",Permisos!$C33)),"1","0")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G28" t="str">
         <f>IF(ISNUMBER(SEARCH("create",Permisos!$C33)),"1","0")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H28" t="str">
         <f>IF(ISNUMBER(SEARCH("unlink",Permisos!$C33)),"1","0")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
-        <f>CONCATENATE("access_",Permisos!B31,"_for_","group_name_",Permisos!D33)</f>
-        <v>access_vehicle_for_group_name_</v>
+        <f>CONCATENATE("access_",Permisos!B34,"_for_","group_name_",Permisos!D34)</f>
+        <v>access_exchange_cotizacion_dolar_bcra_for_group_name_exchange_administrator</v>
       </c>
       <c r="B29" t="str">
-        <f>CONCATENATE(Permisos!B31,"_for_",Permisos!D33)</f>
-        <v>vehicle_for_</v>
+        <f>CONCATENATE(Permisos!B34,"_for_",Permisos!D34)</f>
+        <v>exchange_cotizacion_dolar_bcra_for_exchange_administrator</v>
       </c>
       <c r="C29" t="str">
         <f>CONCATENATE("model_",Permisos!B34)</f>
-        <v>model_vehicle_status</v>
+        <v>model_exchange_cotizacion_dolar_bcra</v>
       </c>
       <c r="D29" t="str">
-        <f>CONCATENATE("group_name_",Permisos!D33)</f>
-        <v>group_name_</v>
+        <f>CONCATENATE("group_name_",Permisos!D34)</f>
+        <v>group_name_exchange_administrator</v>
       </c>
       <c r="E29" t="str">
         <f>IF(ISNUMBER(SEARCH("read",Permisos!$C34)),"1","0")</f>
@@ -2057,20 +2186,20 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
-        <f>CONCATENATE("access_",Permisos!B32,"_for_","group_name_",Permisos!D34)</f>
-        <v>access_vehicle_model_for_group_name_</v>
+        <f>CONCATENATE("access_",Permisos!B35,"_for_","group_name_",Permisos!D35)</f>
+        <v>access_exchange_cotizacion_dolar_bcra_for_group_name_solo_lectura</v>
       </c>
       <c r="B30" t="str">
-        <f>CONCATENATE(Permisos!B32,"_for_",Permisos!D34)</f>
-        <v>vehicle_model_for_</v>
+        <f>CONCATENATE(Permisos!B35,"_for_",Permisos!D35)</f>
+        <v>exchange_cotizacion_dolar_bcra_for_solo_lectura</v>
       </c>
       <c r="C30" t="str">
         <f>CONCATENATE("model_",Permisos!B35)</f>
-        <v>model_res_partner</v>
+        <v>model_exchange_cotizacion_dolar_bcra</v>
       </c>
       <c r="D30" t="str">
-        <f>CONCATENATE("group_name_",Permisos!D34)</f>
-        <v>group_name_</v>
+        <f>CONCATENATE("group_name_",Permisos!D35)</f>
+        <v>group_name_solo_lectura</v>
       </c>
       <c r="E30" t="str">
         <f>IF(ISNUMBER(SEARCH("read",Permisos!$C35)),"1","0")</f>
@@ -2078,33 +2207,33 @@
       </c>
       <c r="F30" t="str">
         <f>IF(ISNUMBER(SEARCH("write",Permisos!$C35)),"1","0")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G30" t="str">
         <f>IF(ISNUMBER(SEARCH("create",Permisos!$C35)),"1","0")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H30" t="str">
         <f>IF(ISNUMBER(SEARCH("unlink",Permisos!$C35)),"1","0")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
-        <f>CONCATENATE("access_",Permisos!B33,"_for_","group_name_",Permisos!D35)</f>
-        <v>access_vehicle_color_for_group_name_</v>
+        <f>CONCATENATE("access_",Permisos!B36,"_for_","group_name_",Permisos!D36)</f>
+        <v>access_exchange_cotizacion_dolar_bcra_for_group_name_exchange_administracion</v>
       </c>
       <c r="B31" t="str">
-        <f>CONCATENATE(Permisos!B33,"_for_",Permisos!D35)</f>
-        <v>vehicle_color_for_</v>
+        <f>CONCATENATE(Permisos!B36,"_for_",Permisos!D36)</f>
+        <v>exchange_cotizacion_dolar_bcra_for_exchange_administracion</v>
       </c>
       <c r="C31" t="str">
         <f>CONCATENATE("model_",Permisos!B36)</f>
-        <v>model_config</v>
+        <v>model_exchange_cotizacion_dolar_bcra</v>
       </c>
       <c r="D31" t="str">
-        <f>CONCATENATE("group_name_",Permisos!D35)</f>
-        <v>group_name_</v>
+        <f>CONCATENATE("group_name_",Permisos!D36)</f>
+        <v>group_name_exchange_administracion</v>
       </c>
       <c r="E31" t="str">
         <f>IF(ISNUMBER(SEARCH("read",Permisos!$C36)),"1","0")</f>
@@ -2120,24 +2249,24 @@
       </c>
       <c r="H31" t="str">
         <f>IF(ISNUMBER(SEARCH("unlink",Permisos!$C36)),"1","0")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
-        <f>CONCATENATE("access_",Permisos!B34,"_for_","group_name_",Permisos!D36)</f>
-        <v>access_vehicle_status_for_group_name_</v>
+        <f>CONCATENATE("access_",Permisos!B37,"_for_","group_name_",Permisos!D37)</f>
+        <v>access__for_group_name_</v>
       </c>
       <c r="B32" t="str">
-        <f>CONCATENATE(Permisos!B34,"_for_",Permisos!D36)</f>
-        <v>vehicle_status_for_</v>
+        <f>CONCATENATE(Permisos!B37,"_for_",Permisos!D37)</f>
+        <v>_for_</v>
       </c>
       <c r="C32" t="str">
         <f>CONCATENATE("model_",Permisos!B37)</f>
         <v>model_</v>
       </c>
       <c r="D32" t="str">
-        <f>CONCATENATE("group_name_",Permisos!D36)</f>
+        <f>CONCATENATE("group_name_",Permisos!D37)</f>
         <v>group_name_</v>
       </c>
       <c r="E32" t="str">
@@ -2159,8 +2288,8 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
-        <f>CONCATENATE("access_",Permisos!B38,"_for_","group_name_",Permisos!D38)</f>
-        <v>access__for_group_name_</v>
+        <f>CONCATENATE("access_",Permisos!B35,"_for_","group_name_",Permisos!D37)</f>
+        <v>access_exchange_cotizacion_dolar_bcra_for_group_name_</v>
       </c>
       <c r="B33" t="str">
         <f>CONCATENATE(Permisos!B38,"_for_",Permisos!D38)</f>
@@ -2193,8 +2322,8 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
-        <f>CONCATENATE("access_",Permisos!B39,"_for_","group_name_",Permisos!D39)</f>
-        <v>access__for_group_name_</v>
+        <f>CONCATENATE("access_",Permisos!B36,"_for_","group_name_",Permisos!D38)</f>
+        <v>access_exchange_cotizacion_dolar_bcra_for_group_name_</v>
       </c>
       <c r="B34" t="str">
         <f>CONCATENATE(Permisos!B39,"_for_",Permisos!D39)</f>
@@ -2227,12 +2356,12 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
-        <f>CONCATENATE("access_",Permisos!B35,"_for_","group_name_",Permisos!D40)</f>
-        <v>access_res_partner_for_group_name_</v>
+        <f>CONCATENATE("access_",Permisos!B37,"_for_","group_name_",Permisos!D39)</f>
+        <v>access__for_group_name_</v>
       </c>
       <c r="B35" t="str">
         <f>CONCATENATE(Permisos!B35,"_for_",Permisos!D40)</f>
-        <v>res_partner_for_</v>
+        <v>exchange_cotizacion_dolar_bcra_for_</v>
       </c>
       <c r="C35" t="str">
         <f>CONCATENATE("model_",Permisos!B40)</f>
@@ -2261,12 +2390,12 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
-        <f>CONCATENATE("access_",Permisos!B36,"_for_","group_name_",Permisos!D41)</f>
-        <v>access_config_for_group_name_</v>
+        <f>CONCATENATE("access_",Permisos!B38,"_for_","group_name_",Permisos!D40)</f>
+        <v>access__for_group_name_</v>
       </c>
       <c r="B36" t="str">
         <f>CONCATENATE(Permisos!B36,"_for_",Permisos!D41)</f>
-        <v>config_for_</v>
+        <v>exchange_cotizacion_dolar_bcra_for_</v>
       </c>
       <c r="C36" t="str">
         <f>CONCATENATE("model_",Permisos!B41)</f>
@@ -2295,7 +2424,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
-        <f>CONCATENATE("access_",Permisos!B37,"_for_","group_name_",Permisos!D42)</f>
+        <f>CONCATENATE("access_",Permisos!B39,"_for_","group_name_",Permisos!D41)</f>
         <v>access__for_group_name_</v>
       </c>
       <c r="B37" t="str">
@@ -2329,7 +2458,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
-        <f>CONCATENATE("access_",Permisos!B43,"_for_","group_name_",Permisos!D43)</f>
+        <f>CONCATENATE("access_",Permisos!B40,"_for_","group_name_",Permisos!D42)</f>
         <v>access__for_group_name_</v>
       </c>
       <c r="B38" t="str">

</xml_diff>